<commit_message>
Maybe...? Got it working?
</commit_message>
<xml_diff>
--- a/Projects/Project_4/Alpha_Time_Relationship.xlsx
+++ b/Projects/Project_4/Alpha_Time_Relationship.xlsx
@@ -8,23 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksonrankin/Desktop/Student/7/PH385/Projects/Project_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7B97DD-E9F2-924C-AD2F-D9BE6273B6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D9B4B9-42A6-654F-B44A-A2C932AD790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="880" windowWidth="28040" windowHeight="16940" xr2:uid="{23DE14DE-8941-ED4E-AA39-B14B5B9DBBDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$3:$B$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$3:$C$13</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$B$3:$B$13</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$C$2</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$C$3:$C$13</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -84,7 +74,7 @@
     <t>5474.5876 ms</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>Took over 100,000 iters. Did not complete</t>
   </si>
 </sst>
 </file>
@@ -459,12 +449,12 @@
   <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>